<commit_message>
Fix column names and handle special cases in file processing
</commit_message>
<xml_diff>
--- a/input_data/data_errors_3/valores.xlsx
+++ b/input_data/data_errors_3/valores.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
-    <t xml:space="preserve">id</t>
+    <t xml:space="preserve">codigo</t>
   </si>
   <si>
     <t xml:space="preserve">nome</t>
@@ -426,10 +426,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="24.58"/>

</xml_diff>